<commit_message>
fix: ajustes na tela de Novo Pedido (checkboxes alinhadas, busca por código, normalização do cilíndrico)
</commit_message>
<xml_diff>
--- a/Nova pasta/pagamentos_2025-09-06.xlsx
+++ b/Nova pasta/pagamentos_2025-09-06.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,12 +498,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SHINEDUX</t>
+          <t>PEREGO</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BVS 1.61 AR</t>
+          <t>ULTEX INCOLOR</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -513,7 +513,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Base 4.00 / Adição +1.50</t>
+          <t>Base 4.00 / Adição +2.50</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -522,18 +522,18 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SHINEDUX</t>
+          <t>PEREGO</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BVS 1.61 AR</t>
+          <t>ULTEX INCOLOR</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
@@ -573,7 +573,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Base 6.00 / Adição +2.50</t>
+          <t>Base 4.00 / Adição +2.50</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -593,47 +593,107 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>BVS 1.61 AR</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Base 6.00 / Adição +2.50</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SHINEDUX</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>BVS 1.67 AR BLUE</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Base 4.00 / Adição +3.00</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Base 4.00 / Adição +1.50</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>2025-09-06</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" s="1" t="inlineStr">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SHINEDUX</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BVS 1.67 AR BLUE</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Base 6.00 / Adição +1.50</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" s="1" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="F10" s="1" t="n">
         <v>243</v>
       </c>
     </row>

</xml_diff>